<commit_message>
Fixed GNFR spreading + tests
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/id_nummers.xlsx
+++ b/logic/test/data/_input/05_model_parameters/id_nummers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\projects\E-MAP\05_Runs\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906BA0ED-C829-48F5-8654-BCC5BC96BB24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55B591AF-7BFD-4383-B53E-5319A164A9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6FB3B743-6D47-45BD-BADE-A392A55C90C7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6FB3B743-6D47-45BD-BADE-A392A55C90C7}"/>
   </bookViews>
   <sheets>
     <sheet name="NFR" sheetId="3" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="464">
   <si>
     <t>GNFR_code</t>
   </si>
@@ -1450,6 +1450,12 @@
   </si>
   <si>
     <t>Road transport: Resuspension</t>
+  </si>
+  <si>
+    <t>1A3di(i)</t>
+  </si>
+  <si>
+    <t>International maritime navigation</t>
   </si>
 </sst>
 </file>
@@ -1530,8 +1536,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F4DD3638-9D35-451E-BDC2-2F2772496E0E}" name="tbl_GNFR4" displayName="tbl_GNFR4" ref="A1:E129" totalsRowShown="0">
-  <autoFilter ref="A1:E129" xr:uid="{5A4366AA-9896-4273-8005-230DCB1C6B2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F4DD3638-9D35-451E-BDC2-2F2772496E0E}" name="tbl_GNFR4" displayName="tbl_GNFR4" ref="A1:E130" totalsRowShown="0">
+  <autoFilter ref="A1:E130" xr:uid="{5A4366AA-9896-4273-8005-230DCB1C6B2F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E130">
+    <sortCondition ref="A1:A130"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="2" xr3:uid="{457DE52E-AE84-48F5-B99B-134CA848C6C3}" name="NFR_code"/>
     <tableColumn id="1" xr3:uid="{3F707F06-E2DF-4782-973E-B9DEE5B38E0A}" name="NFR_number"/>
@@ -1884,21 +1893,21 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A106" workbookViewId="0">
-      <selection sqref="A1:B129"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="109.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>284</v>
       </c>
@@ -1915,7 +1924,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1932,7 +1941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1949,7 +1958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1966,7 +1975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1983,7 +1992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2000,7 +2009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2017,7 +2026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2034,7 +2043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2051,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -2068,7 +2077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -2085,7 +2094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2102,7 +2111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2119,7 +2128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2136,7 +2145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -2153,7 +2162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2170,7 +2179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -2187,7 +2196,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2204,7 +2213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2238,7 +2247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2255,12 +2264,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>460</v>
       </c>
       <c r="B22">
-        <v>7128</v>
+        <v>7021</v>
       </c>
       <c r="C22" t="s">
         <v>461</v>
@@ -2272,12 +2281,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
       <c r="B23">
-        <v>7021</v>
+        <v>7022</v>
       </c>
       <c r="C23" t="s">
         <v>176</v>
@@ -2289,66 +2298,66 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>462</v>
       </c>
       <c r="B24">
-        <v>7022</v>
+        <v>7023</v>
       </c>
       <c r="C24" t="s">
-        <v>177</v>
+        <v>463</v>
       </c>
       <c r="D24" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25">
-        <v>7023</v>
+        <v>7024</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26">
+        <v>7025</v>
+      </c>
+      <c r="C26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" t="s">
+        <v>457</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>52</v>
       </c>
-      <c r="B26">
-        <v>7024</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B27">
+        <v>7026</v>
+      </c>
+      <c r="C27" t="s">
         <v>179</v>
-      </c>
-      <c r="D26" t="s">
-        <v>457</v>
-      </c>
-      <c r="E26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27">
-        <v>7025</v>
-      </c>
-      <c r="C27" t="s">
-        <v>180</v>
       </c>
       <c r="D27" t="s">
         <v>457</v>
@@ -2357,117 +2366,117 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28">
+        <v>7027</v>
+      </c>
+      <c r="C28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D28" t="s">
+        <v>457</v>
+      </c>
+      <c r="E28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>54</v>
       </c>
-      <c r="B28">
-        <v>7026</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B29">
+        <v>7028</v>
+      </c>
+      <c r="C29" t="s">
         <v>181</v>
       </c>
-      <c r="D28" t="s">
-        <v>457</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D29" t="s">
+        <v>457</v>
+      </c>
+      <c r="E29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B29">
-        <v>7027</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B30">
+        <v>7029</v>
+      </c>
+      <c r="C30" t="s">
         <v>182</v>
       </c>
-      <c r="D29" t="s">
-        <v>457</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D30" t="s">
+        <v>457</v>
+      </c>
+      <c r="E30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>56</v>
       </c>
-      <c r="B30">
-        <v>7028</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B31">
+        <v>7030</v>
+      </c>
+      <c r="C31" t="s">
         <v>183</v>
       </c>
-      <c r="D30" t="s">
-        <v>457</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" t="s">
+        <v>457</v>
+      </c>
+      <c r="E31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>57</v>
       </c>
-      <c r="B31">
-        <v>7029</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B32">
+        <v>7031</v>
+      </c>
+      <c r="C32" t="s">
         <v>184</v>
       </c>
-      <c r="D31" t="s">
-        <v>457</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D32" t="s">
+        <v>457</v>
+      </c>
+      <c r="E32" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>58</v>
       </c>
-      <c r="B32">
-        <v>7030</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B33">
+        <v>7032</v>
+      </c>
+      <c r="C33" t="s">
         <v>185</v>
       </c>
-      <c r="D32" t="s">
-        <v>457</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D33" t="s">
+        <v>457</v>
+      </c>
+      <c r="E33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>59</v>
       </c>
-      <c r="B33">
-        <v>7031</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B34">
+        <v>7033</v>
+      </c>
+      <c r="C34" t="s">
         <v>186</v>
-      </c>
-      <c r="D33" t="s">
-        <v>457</v>
-      </c>
-      <c r="E33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34">
-        <v>7032</v>
-      </c>
-      <c r="C34" t="s">
-        <v>187</v>
       </c>
       <c r="D34" t="s">
         <v>457</v>
@@ -2476,66 +2485,66 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35">
+        <v>7034</v>
+      </c>
+      <c r="C35" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" t="s">
+        <v>457</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>61</v>
       </c>
-      <c r="B35">
-        <v>7033</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B36">
+        <v>7035</v>
+      </c>
+      <c r="C36" t="s">
         <v>188</v>
       </c>
-      <c r="D35" t="s">
-        <v>457</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
+        <v>457</v>
+      </c>
+      <c r="E36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>62</v>
       </c>
-      <c r="B36">
-        <v>7034</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B37">
+        <v>7036</v>
+      </c>
+      <c r="C37" t="s">
         <v>189</v>
       </c>
-      <c r="D36" t="s">
-        <v>457</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D37" t="s">
+        <v>457</v>
+      </c>
+      <c r="E37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>63</v>
       </c>
-      <c r="B37">
-        <v>7035</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B38">
+        <v>7037</v>
+      </c>
+      <c r="C38" t="s">
         <v>190</v>
-      </c>
-      <c r="D37" t="s">
-        <v>457</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38">
-        <v>7036</v>
-      </c>
-      <c r="C38" t="s">
-        <v>191</v>
       </c>
       <c r="D38" t="s">
         <v>457</v>
@@ -2544,15 +2553,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B39">
-        <v>7037</v>
+        <v>7038</v>
       </c>
       <c r="C39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D39" t="s">
         <v>457</v>
@@ -2561,15 +2570,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40">
-        <v>7038</v>
+        <v>7039</v>
       </c>
       <c r="C40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D40" t="s">
         <v>457</v>
@@ -2578,15 +2587,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41">
-        <v>7039</v>
+        <v>7040</v>
       </c>
       <c r="C41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D41" t="s">
         <v>457</v>
@@ -2595,15 +2604,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42">
-        <v>7040</v>
+        <v>7041</v>
       </c>
       <c r="C42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D42" t="s">
         <v>457</v>
@@ -2612,15 +2621,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43">
-        <v>7041</v>
+        <v>7042</v>
       </c>
       <c r="C43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D43" t="s">
         <v>457</v>
@@ -2629,15 +2638,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44">
-        <v>7042</v>
+        <v>7043</v>
       </c>
       <c r="C44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D44" t="s">
         <v>457</v>
@@ -2646,15 +2655,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45">
-        <v>7043</v>
+        <v>7044</v>
       </c>
       <c r="C45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D45" t="s">
         <v>457</v>
@@ -2663,32 +2672,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46">
+        <v>7045</v>
+      </c>
+      <c r="C46" t="s">
+        <v>198</v>
+      </c>
+      <c r="D46" t="s">
+        <v>457</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>72</v>
       </c>
-      <c r="B46">
-        <v>7044</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B47">
+        <v>7046</v>
+      </c>
+      <c r="C47" t="s">
         <v>199</v>
-      </c>
-      <c r="D46" t="s">
-        <v>457</v>
-      </c>
-      <c r="E46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47">
-        <v>7045</v>
-      </c>
-      <c r="C47" t="s">
-        <v>200</v>
       </c>
       <c r="D47" t="s">
         <v>457</v>
@@ -2697,15 +2706,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48">
-        <v>7046</v>
+        <v>7047</v>
       </c>
       <c r="C48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D48" t="s">
         <v>457</v>
@@ -2714,15 +2723,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49">
-        <v>7047</v>
+        <v>7048</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D49" t="s">
         <v>457</v>
@@ -2731,15 +2740,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50">
-        <v>7048</v>
+        <v>7049</v>
       </c>
       <c r="C50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D50" t="s">
         <v>457</v>
@@ -2748,15 +2757,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51">
-        <v>7049</v>
+        <v>7050</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D51" t="s">
         <v>457</v>
@@ -2765,15 +2774,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52">
-        <v>7050</v>
+        <v>7051</v>
       </c>
       <c r="C52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D52" t="s">
         <v>457</v>
@@ -2782,15 +2791,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53">
-        <v>7051</v>
+        <v>7052</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D53" t="s">
         <v>457</v>
@@ -2799,15 +2808,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B54">
-        <v>7057</v>
+        <v>7053</v>
       </c>
       <c r="C54" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D54" t="s">
         <v>457</v>
@@ -2816,15 +2825,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B55">
-        <v>7058</v>
+        <v>7054</v>
       </c>
       <c r="C55" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D55" t="s">
         <v>457</v>
@@ -2833,15 +2842,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B56">
-        <v>7052</v>
+        <v>7055</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D56" t="s">
         <v>457</v>
@@ -2850,15 +2859,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57">
-        <v>7053</v>
+        <v>7056</v>
       </c>
       <c r="C57" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D57" t="s">
         <v>457</v>
@@ -2867,15 +2876,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58">
-        <v>7054</v>
+        <v>7057</v>
       </c>
       <c r="C58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D58" t="s">
         <v>457</v>
@@ -2884,15 +2893,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B59">
-        <v>7055</v>
+        <v>7058</v>
       </c>
       <c r="C59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D59" t="s">
         <v>457</v>
@@ -2901,15 +2910,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B60">
-        <v>7056</v>
+        <v>7059</v>
       </c>
       <c r="C60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D60" t="s">
         <v>457</v>
@@ -2918,15 +2927,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B61">
-        <v>7059</v>
+        <v>7060</v>
       </c>
       <c r="C61" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D61" t="s">
         <v>457</v>
@@ -2935,15 +2944,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62">
-        <v>7060</v>
+        <v>7061</v>
       </c>
       <c r="C62" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D62" t="s">
         <v>457</v>
@@ -2952,15 +2961,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63">
-        <v>7061</v>
+        <v>7062</v>
       </c>
       <c r="C63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D63" t="s">
         <v>457</v>
@@ -2969,15 +2978,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B64">
-        <v>7062</v>
+        <v>7063</v>
       </c>
       <c r="C64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D64" t="s">
         <v>457</v>
@@ -2986,15 +2995,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B65">
-        <v>7063</v>
+        <v>7064</v>
       </c>
       <c r="C65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D65" t="s">
         <v>457</v>
@@ -3003,15 +3012,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66">
-        <v>7064</v>
+        <v>7065</v>
       </c>
       <c r="C66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D66" t="s">
         <v>457</v>
@@ -3020,15 +3029,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67">
-        <v>7065</v>
+        <v>7066</v>
       </c>
       <c r="C67" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D67" t="s">
         <v>457</v>
@@ -3037,15 +3046,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B68">
-        <v>7066</v>
+        <v>7067</v>
       </c>
       <c r="C68" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D68" t="s">
         <v>457</v>
@@ -3054,15 +3063,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B69">
-        <v>7067</v>
+        <v>7068</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D69" t="s">
         <v>457</v>
@@ -3071,15 +3080,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B70">
-        <v>7068</v>
+        <v>7069</v>
       </c>
       <c r="C70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D70" t="s">
         <v>457</v>
@@ -3088,49 +3097,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71">
+        <v>7070</v>
+      </c>
+      <c r="C71" t="s">
+        <v>223</v>
+      </c>
+      <c r="D71" t="s">
+        <v>457</v>
+      </c>
+      <c r="E71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>97</v>
       </c>
-      <c r="B71">
-        <v>7069</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B72">
+        <v>7071</v>
+      </c>
+      <c r="C72" t="s">
         <v>224</v>
       </c>
-      <c r="D71" t="s">
-        <v>457</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="D72" t="s">
+        <v>457</v>
+      </c>
+      <c r="E72" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>98</v>
       </c>
-      <c r="B72">
-        <v>7070</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B73">
+        <v>7072</v>
+      </c>
+      <c r="C73" t="s">
         <v>225</v>
-      </c>
-      <c r="D72" t="s">
-        <v>457</v>
-      </c>
-      <c r="E72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>99</v>
-      </c>
-      <c r="B73">
-        <v>7071</v>
-      </c>
-      <c r="C73" t="s">
-        <v>226</v>
       </c>
       <c r="D73" t="s">
         <v>457</v>
@@ -3139,32 +3148,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74">
+        <v>7073</v>
+      </c>
+      <c r="C74" t="s">
+        <v>226</v>
+      </c>
+      <c r="D74" t="s">
+        <v>457</v>
+      </c>
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>100</v>
       </c>
-      <c r="B74">
-        <v>7072</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B75">
+        <v>7074</v>
+      </c>
+      <c r="C75" t="s">
         <v>227</v>
-      </c>
-      <c r="D74" t="s">
-        <v>457</v>
-      </c>
-      <c r="E74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>101</v>
-      </c>
-      <c r="B75">
-        <v>7073</v>
-      </c>
-      <c r="C75" t="s">
-        <v>228</v>
       </c>
       <c r="D75" t="s">
         <v>457</v>
@@ -3173,15 +3182,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B76">
-        <v>7074</v>
+        <v>7075</v>
       </c>
       <c r="C76" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D76" t="s">
         <v>457</v>
@@ -3190,15 +3199,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B77">
-        <v>7075</v>
+        <v>7076</v>
       </c>
       <c r="C77" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D77" t="s">
         <v>457</v>
@@ -3207,15 +3216,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B78">
-        <v>7076</v>
+        <v>7077</v>
       </c>
       <c r="C78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D78" t="s">
         <v>457</v>
@@ -3224,15 +3233,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B79">
-        <v>7077</v>
+        <v>7078</v>
       </c>
       <c r="C79" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D79" t="s">
         <v>457</v>
@@ -3241,15 +3250,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B80">
-        <v>7078</v>
+        <v>7079</v>
       </c>
       <c r="C80" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D80" t="s">
         <v>457</v>
@@ -3258,32 +3267,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81">
+        <v>7080</v>
+      </c>
+      <c r="C81" t="s">
+        <v>233</v>
+      </c>
+      <c r="D81" t="s">
+        <v>457</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>107</v>
       </c>
-      <c r="B81">
-        <v>7079</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="B82">
+        <v>7081</v>
+      </c>
+      <c r="C82" t="s">
         <v>234</v>
-      </c>
-      <c r="D81" t="s">
-        <v>457</v>
-      </c>
-      <c r="E81" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>108</v>
-      </c>
-      <c r="B82">
-        <v>7080</v>
-      </c>
-      <c r="C82" t="s">
-        <v>235</v>
       </c>
       <c r="D82" t="s">
         <v>457</v>
@@ -3292,15 +3301,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B83">
-        <v>7081</v>
+        <v>7082</v>
       </c>
       <c r="C83" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D83" t="s">
         <v>457</v>
@@ -3309,15 +3318,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B84">
-        <v>7082</v>
+        <v>7083</v>
       </c>
       <c r="C84" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D84" t="s">
         <v>457</v>
@@ -3326,15 +3335,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B85">
-        <v>7083</v>
+        <v>7084</v>
       </c>
       <c r="C85" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D85" t="s">
         <v>457</v>
@@ -3343,15 +3352,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86">
-        <v>7084</v>
+        <v>7085</v>
       </c>
       <c r="C86" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D86" t="s">
         <v>457</v>
@@ -3360,15 +3369,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B87">
-        <v>7085</v>
+        <v>7086</v>
       </c>
       <c r="C87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D87" t="s">
         <v>457</v>
@@ -3377,32 +3386,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>113</v>
+      </c>
+      <c r="B88">
+        <v>7087</v>
+      </c>
+      <c r="C88" t="s">
+        <v>240</v>
+      </c>
+      <c r="D88" t="s">
+        <v>457</v>
+      </c>
+      <c r="E88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>114</v>
       </c>
-      <c r="B88">
-        <v>7086</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="B89">
+        <v>7088</v>
+      </c>
+      <c r="C89" t="s">
         <v>241</v>
-      </c>
-      <c r="D88" t="s">
-        <v>457</v>
-      </c>
-      <c r="E88" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>115</v>
-      </c>
-      <c r="B89">
-        <v>7087</v>
-      </c>
-      <c r="C89" t="s">
-        <v>242</v>
       </c>
       <c r="D89" t="s">
         <v>457</v>
@@ -3411,15 +3420,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B90">
-        <v>7088</v>
+        <v>7089</v>
       </c>
       <c r="C90" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D90" t="s">
         <v>457</v>
@@ -3428,15 +3437,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B91">
-        <v>7089</v>
+        <v>7090</v>
       </c>
       <c r="C91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D91" t="s">
         <v>457</v>
@@ -3445,15 +3454,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B92">
-        <v>7090</v>
+        <v>7091</v>
       </c>
       <c r="C92" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D92" t="s">
         <v>457</v>
@@ -3462,15 +3471,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B93">
-        <v>7091</v>
+        <v>7092</v>
       </c>
       <c r="C93" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D93" t="s">
         <v>457</v>
@@ -3479,15 +3488,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B94">
-        <v>7092</v>
+        <v>7093</v>
       </c>
       <c r="C94" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D94" t="s">
         <v>457</v>
@@ -3496,15 +3505,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B95">
-        <v>7093</v>
+        <v>7094</v>
       </c>
       <c r="C95" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D95" t="s">
         <v>457</v>
@@ -3513,15 +3522,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B96">
-        <v>7094</v>
+        <v>7095</v>
       </c>
       <c r="C96" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D96" t="s">
         <v>457</v>
@@ -3530,15 +3539,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B97">
-        <v>7095</v>
+        <v>7096</v>
       </c>
       <c r="C97" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D97" t="s">
         <v>457</v>
@@ -3547,15 +3556,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B98">
-        <v>7096</v>
+        <v>7097</v>
       </c>
       <c r="C98" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D98" t="s">
         <v>457</v>
@@ -3564,15 +3573,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B99">
-        <v>7097</v>
+        <v>7098</v>
       </c>
       <c r="C99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D99" t="s">
         <v>457</v>
@@ -3581,15 +3590,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B100">
-        <v>7098</v>
+        <v>7099</v>
       </c>
       <c r="C100" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D100" t="s">
         <v>457</v>
@@ -3598,32 +3607,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>126</v>
+      </c>
+      <c r="B101">
+        <v>7100</v>
+      </c>
+      <c r="C101" t="s">
+        <v>253</v>
+      </c>
+      <c r="D101" t="s">
+        <v>457</v>
+      </c>
+      <c r="E101" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>127</v>
       </c>
-      <c r="B101">
-        <v>7099</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="B102">
+        <v>7101</v>
+      </c>
+      <c r="C102" t="s">
         <v>254</v>
-      </c>
-      <c r="D101" t="s">
-        <v>457</v>
-      </c>
-      <c r="E101" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>128</v>
-      </c>
-      <c r="B102">
-        <v>7100</v>
-      </c>
-      <c r="C102" t="s">
-        <v>255</v>
       </c>
       <c r="D102" t="s">
         <v>457</v>
@@ -3632,15 +3641,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B103">
-        <v>7101</v>
+        <v>7102</v>
       </c>
       <c r="C103" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D103" t="s">
         <v>457</v>
@@ -3649,15 +3658,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B104">
-        <v>7102</v>
+        <v>7103</v>
       </c>
       <c r="C104" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D104" t="s">
         <v>457</v>
@@ -3666,15 +3675,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B105">
-        <v>7103</v>
+        <v>7104</v>
       </c>
       <c r="C105" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D105" t="s">
         <v>457</v>
@@ -3683,15 +3692,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B106">
-        <v>7104</v>
+        <v>7105</v>
       </c>
       <c r="C106" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D106" t="s">
         <v>457</v>
@@ -3700,15 +3709,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B107">
-        <v>7105</v>
+        <v>7106</v>
       </c>
       <c r="C107" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D107" t="s">
         <v>457</v>
@@ -3717,15 +3726,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B108">
-        <v>7106</v>
+        <v>7107</v>
       </c>
       <c r="C108" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D108" t="s">
         <v>457</v>
@@ -3734,15 +3743,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B109">
-        <v>7107</v>
+        <v>7108</v>
       </c>
       <c r="C109" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D109" t="s">
         <v>457</v>
@@ -3751,15 +3760,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B110">
-        <v>7108</v>
+        <v>7109</v>
       </c>
       <c r="C110" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D110" t="s">
         <v>457</v>
@@ -3768,15 +3777,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B111">
-        <v>7109</v>
+        <v>7110</v>
       </c>
       <c r="C111" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D111" t="s">
         <v>457</v>
@@ -3785,15 +3794,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B112">
-        <v>7110</v>
+        <v>7111</v>
       </c>
       <c r="C112" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D112" t="s">
         <v>457</v>
@@ -3802,15 +3811,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B113">
-        <v>7111</v>
+        <v>7112</v>
       </c>
       <c r="C113" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D113" t="s">
         <v>457</v>
@@ -3819,32 +3828,32 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>139</v>
+      </c>
+      <c r="B114">
+        <v>7113</v>
+      </c>
+      <c r="C114" t="s">
+        <v>266</v>
+      </c>
+      <c r="D114" t="s">
+        <v>457</v>
+      </c>
+      <c r="E114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>140</v>
       </c>
-      <c r="B114">
-        <v>7112</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="B115">
+        <v>7114</v>
+      </c>
+      <c r="C115" t="s">
         <v>267</v>
-      </c>
-      <c r="D114" t="s">
-        <v>457</v>
-      </c>
-      <c r="E114" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>141</v>
-      </c>
-      <c r="B115">
-        <v>7113</v>
-      </c>
-      <c r="C115" t="s">
-        <v>268</v>
       </c>
       <c r="D115" t="s">
         <v>457</v>
@@ -3853,15 +3862,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B116">
-        <v>7114</v>
+        <v>7115</v>
       </c>
       <c r="C116" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D116" t="s">
         <v>457</v>
@@ -3870,15 +3879,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B117">
-        <v>7115</v>
+        <v>7116</v>
       </c>
       <c r="C117" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D117" t="s">
         <v>457</v>
@@ -3887,15 +3896,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B118">
-        <v>7116</v>
+        <v>7117</v>
       </c>
       <c r="C118" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D118" t="s">
         <v>457</v>
@@ -3904,15 +3913,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B119">
-        <v>7117</v>
+        <v>7118</v>
       </c>
       <c r="C119" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D119" t="s">
         <v>457</v>
@@ -3921,15 +3930,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B120">
-        <v>7118</v>
+        <v>7119</v>
       </c>
       <c r="C120" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D120" t="s">
         <v>457</v>
@@ -3938,15 +3947,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B121">
-        <v>7119</v>
+        <v>7120</v>
       </c>
       <c r="C121" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D121" t="s">
         <v>457</v>
@@ -3955,15 +3964,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B122">
-        <v>7120</v>
+        <v>7121</v>
       </c>
       <c r="C122" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D122" t="s">
         <v>457</v>
@@ -3972,15 +3981,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B123">
-        <v>7121</v>
+        <v>7122</v>
       </c>
       <c r="C123" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D123" t="s">
         <v>457</v>
@@ -3989,15 +3998,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B124">
-        <v>7122</v>
+        <v>7123</v>
       </c>
       <c r="C124" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D124" t="s">
         <v>457</v>
@@ -4006,15 +4015,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B125">
-        <v>7123</v>
+        <v>7124</v>
       </c>
       <c r="C125" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D125" t="s">
         <v>457</v>
@@ -4023,15 +4032,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B126">
-        <v>7124</v>
+        <v>7125</v>
       </c>
       <c r="C126" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D126" t="s">
         <v>457</v>
@@ -4040,15 +4049,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B127">
-        <v>7125</v>
+        <v>7126</v>
       </c>
       <c r="C127" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D127" t="s">
         <v>457</v>
@@ -4057,15 +4066,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B128">
-        <v>7126</v>
+        <v>7127</v>
       </c>
       <c r="C128" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D128" t="s">
         <v>457</v>
@@ -4074,27 +4083,45 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129">
+        <v>7128</v>
+      </c>
+      <c r="C129" t="s">
+        <v>281</v>
+      </c>
+      <c r="D129" t="s">
+        <v>457</v>
+      </c>
+      <c r="E129" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>155</v>
       </c>
-      <c r="B129">
-        <v>7127</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="B130">
+        <v>7129</v>
+      </c>
+      <c r="C130" t="s">
         <v>282</v>
       </c>
-      <c r="D129" t="s">
-        <v>457</v>
-      </c>
-      <c r="E129" t="s">
+      <c r="D130" t="s">
+        <v>457</v>
+      </c>
+      <c r="E130" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4107,17 +4134,17 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B1:B14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4131,7 +4158,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4145,7 +4172,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4159,7 +4186,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4173,7 +4200,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4187,7 +4214,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -4201,7 +4228,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4215,7 +4242,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4229,7 +4256,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -4243,7 +4270,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -4257,7 +4284,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4271,7 +4298,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -4285,7 +4312,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4299,7 +4326,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -4328,18 +4355,18 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>341</v>
       </c>
@@ -4350,7 +4377,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4361,7 +4388,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4372,7 +4399,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4383,7 +4410,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4394,7 +4421,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4405,7 +4432,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4416,7 +4443,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4427,7 +4454,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4438,7 +4465,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4449,7 +4476,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4460,7 +4487,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4471,7 +4498,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4482,7 +4509,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4493,7 +4520,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4504,7 +4531,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4515,7 +4542,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4526,7 +4553,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4537,7 +4564,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4548,7 +4575,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4559,7 +4586,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4570,7 +4597,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4581,7 +4608,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4592,7 +4619,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4603,7 +4630,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4614,7 +4641,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4625,7 +4652,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4636,7 +4663,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4666,14 +4693,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>454</v>
       </c>
@@ -4687,7 +4714,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4701,7 +4728,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4715,7 +4742,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4729,7 +4756,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4743,7 +4770,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4757,7 +4784,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4771,7 +4798,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4785,7 +4812,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4799,7 +4826,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4813,7 +4840,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4827,7 +4854,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4841,7 +4868,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4855,7 +4882,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -4869,7 +4896,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>24</v>
       </c>
@@ -4883,7 +4910,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>25</v>
       </c>
@@ -4897,7 +4924,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>26</v>
       </c>
@@ -4911,7 +4938,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>27</v>
       </c>
@@ -4925,7 +4952,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>29</v>
       </c>
@@ -4939,7 +4966,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30</v>
       </c>
@@ -4953,7 +4980,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31</v>
       </c>
@@ -4967,7 +4994,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>32</v>
       </c>
@@ -4981,7 +5008,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>34</v>
       </c>
@@ -4995,7 +5022,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>35</v>
       </c>
@@ -5009,7 +5036,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>36</v>
       </c>
@@ -5023,7 +5050,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>37</v>
       </c>
@@ -5037,7 +5064,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>38</v>
       </c>
@@ -5051,7 +5078,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>39</v>
       </c>
@@ -5065,7 +5092,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>40</v>
       </c>
@@ -5079,7 +5106,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>41</v>
       </c>
@@ -5093,7 +5120,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>42</v>
       </c>
@@ -5107,7 +5134,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>43</v>
       </c>
@@ -5121,7 +5148,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>44</v>
       </c>
@@ -5135,7 +5162,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>45</v>
       </c>
@@ -5149,7 +5176,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>46</v>
       </c>
@@ -5163,7 +5190,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>47</v>
       </c>
@@ -5177,7 +5204,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>48</v>
       </c>
@@ -5191,7 +5218,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>49</v>
       </c>
@@ -5205,7 +5232,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>50</v>
       </c>
@@ -5219,7 +5246,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>51</v>
       </c>
@@ -5233,7 +5260,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>52</v>
       </c>
@@ -5247,7 +5274,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>54</v>
       </c>
@@ -5261,7 +5288,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>55</v>
       </c>
@@ -5275,7 +5302,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>56</v>
       </c>
@@ -5289,7 +5316,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>58</v>
       </c>
@@ -5303,7 +5330,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>60</v>
       </c>
@@ -5317,7 +5344,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>61</v>
       </c>
@@ -5331,7 +5358,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>62</v>
       </c>
@@ -5345,7 +5372,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>63</v>
       </c>
@@ -5359,7 +5386,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>64</v>
       </c>
@@ -5373,7 +5400,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>65</v>
       </c>
@@ -5387,7 +5414,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>66</v>
       </c>
@@ -5401,7 +5428,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>67</v>
       </c>
@@ -5415,7 +5442,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>68</v>
       </c>
@@ -5429,7 +5456,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>69</v>
       </c>
@@ -5443,7 +5470,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Support EEZ type for sectors in run configuration
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/id_nummers.xlsx
+++ b/logic/test/data/_input/05_model_parameters/id_nummers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\projects\E-MAP\05_Runs\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55B591AF-7BFD-4383-B53E-5319A164A9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1126A883-2826-4FFC-B919-78F261EF5646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6FB3B743-6D47-45BD-BADE-A392A55C90C7}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="465">
   <si>
     <t>GNFR_code</t>
   </si>
@@ -1456,6 +1456,9 @@
   </si>
   <si>
     <t>International maritime navigation</t>
+  </si>
+  <si>
+    <t>EEZ</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1898,8 @@
   </sheetPr>
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,7 +2329,7 @@
         <v>177</v>
       </c>
       <c r="D25" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2496,7 +2499,7 @@
         <v>187</v>
       </c>
       <c r="D35" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>

</xml_diff>